<commit_message>
added tests for calcrules 2, 17, 18 policy layer with share and ded
</commit_message>
<xml_diff>
--- a/ftest/data/fm31/Worked example policy calculation_MinandMaxdeductibles.xlsx
+++ b/ftest/data/fm31/Worked example policy calculation_MinandMaxdeductibles.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cygwin64\home\Joh\git\ktest\ftest\data\fm31\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{859AD9CB-B3AE-4B79-BE07-1FBEAAC1287B}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{4C5D3269-FF2B-4EBA-960D-C002D9944A7B}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23016" windowHeight="5652" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Worked examples" sheetId="10" r:id="rId1"/>
@@ -128,9 +128,6 @@
   </si>
   <si>
     <t>S5 = S4 + S3 - S5</t>
-  </si>
-  <si>
-    <t>Min deductibles</t>
   </si>
   <si>
     <t>Policy minimum deductible</t>
@@ -194,6 +191,9 @@
       </rPr>
       <t>(Dmax,Min(Max(S3,Dmin),S3+S4)</t>
     </r>
+  </si>
+  <si>
+    <t>Min and Max deductibles</t>
   </si>
 </sst>
 </file>
@@ -981,8 +981,8 @@
   </sheetPr>
   <dimension ref="A1:N44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="L25" sqref="L25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1009,7 +1009,7 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.3">
@@ -1195,10 +1195,10 @@
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12" s="20" t="s">
         <v>37</v>
-      </c>
-      <c r="B12" s="20" t="s">
-        <v>38</v>
       </c>
       <c r="C12" s="28"/>
       <c r="D12" s="28"/>
@@ -1215,10 +1215,10 @@
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="B13" s="20" t="s">
         <v>39</v>
-      </c>
-      <c r="B13" s="20" t="s">
-        <v>40</v>
       </c>
       <c r="C13" s="30"/>
       <c r="D13" s="30"/>
@@ -1426,14 +1426,17 @@
       <c r="I21" s="57"/>
       <c r="J21" s="57"/>
       <c r="K21" s="37"/>
-      <c r="L21" s="23"/>
+      <c r="L21" s="23">
+        <f>SUM(C21:J21)</f>
+        <v>122900</v>
+      </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="B22" s="20" t="s">
         <v>41</v>
-      </c>
-      <c r="B22" s="20" t="s">
-        <v>42</v>
       </c>
       <c r="C22" s="57">
         <f>MIN(C21,C20)</f>
@@ -1479,7 +1482,7 @@
       <c r="J23" s="57"/>
       <c r="K23" s="40"/>
       <c r="L23" s="41">
-        <f>SUM(C23:J23)</f>
+        <f>L21-L22</f>
         <v>54400</v>
       </c>
       <c r="M23" s="42"/>
@@ -1489,7 +1492,7 @@
         <v>30</v>
       </c>
       <c r="B24" s="20" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C24" s="43"/>
       <c r="D24" s="43"/>

</xml_diff>